<commit_message>
XHTML to DT added Username&Password in Config now
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmet.altin\Documents\UiPath\REF_API_CalculateClientSecurityHash\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\REPOS\Renova\UiPath-Personal-Project\REF_API_CalculateClientSecurityHash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4F5368-A02C-4266-9EC2-EEA5FA73C6CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95805AD-4D8E-4CBB-A7BB-E02DADA45F64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -159,13 +159,25 @@
   </si>
   <si>
     <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>asd123@asd.com</t>
+  </si>
+  <si>
+    <t>asd123asd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -189,8 +201,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,6 +219,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -231,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -243,6 +268,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,7 +588,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -642,8 +670,24 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="6"/>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>